<commit_message>
Created a login & logout component in react
</commit_message>
<xml_diff>
--- a/Training Files/Front-End Trainings - Dhilushan.xlsx
+++ b/Training Files/Front-End Trainings - Dhilushan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="206">
   <si>
     <t>HTML5, CSS3, Tailwind CSS (Foundation)</t>
   </si>
@@ -956,7 +956,7 @@
   <dimension ref="A1:G993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1375,7 +1375,9 @@
       <c r="E25" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1391,7 +1393,9 @@
       <c r="E26" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -1407,7 +1411,9 @@
       <c r="E27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>

</xml_diff>

<commit_message>
Updated with all the training files covered until 09-06-2025
</commit_message>
<xml_diff>
--- a/Training Files/Front-End Trainings - Dhilushan.xlsx
+++ b/Training Files/Front-End Trainings - Dhilushan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="206">
   <si>
     <t>HTML5, CSS3, Tailwind CSS (Foundation)</t>
   </si>
@@ -955,8 +955,8 @@
   </sheetPr>
   <dimension ref="A1:G993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1447,7 +1447,9 @@
       <c r="E29" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>

</xml_diff>

<commit_message>
Completed upto contact manager application
</commit_message>
<xml_diff>
--- a/Training Files/Front-End Trainings - Dhilushan.xlsx
+++ b/Training Files/Front-End Trainings - Dhilushan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="206">
   <si>
     <t>HTML5, CSS3, Tailwind CSS (Foundation)</t>
   </si>
@@ -955,8 +955,8 @@
   </sheetPr>
   <dimension ref="A1:G993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1465,7 +1465,9 @@
       <c r="E30" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="6"/>
+      <c r="F30" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>

</xml_diff>

<commit_message>
Completed Dynamic controller app
</commit_message>
<xml_diff>
--- a/Training Files/Front-End Trainings - Dhilushan.xlsx
+++ b/Training Files/Front-End Trainings - Dhilushan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="206">
   <si>
     <t>HTML5, CSS3, Tailwind CSS (Foundation)</t>
   </si>
@@ -955,8 +955,8 @@
   </sheetPr>
   <dimension ref="A1:G993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1529,7 +1529,9 @@
       <c r="E35" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F35" s="6"/>
+      <c r="F35" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>

</xml_diff>